<commit_message>
terminado modal de generar excel
</commit_message>
<xml_diff>
--- a/registros/plantilla/plantilla_registro_atenciones.xlsx
+++ b/registros/plantilla/plantilla_registro_atenciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRM-CARITAS\registros\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED92983B-F8D5-4579-B44A-185A8D153231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85277854-9DB4-4FFB-B41D-C956680CA015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Migrantes" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Asesoría Psicológica</t>
-  </si>
-  <si>
-    <t>Fallecimiento</t>
   </si>
   <si>
     <t>Atención Psicológica</t>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Identificación</t>
+  </si>
+  <si>
+    <t>Falleció</t>
   </si>
 </sst>
 </file>
@@ -333,6 +333,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,21 +355,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="49">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -528,14 +528,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -896,12 +888,12 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{B6B7D83C-BD69-47D7-9B34-4BE22687F3A8}">
-      <tableStyleElement type="wholeTable" dxfId="49"/>
-      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="48"/>
+      <tableStyleElement type="headerRow" dxfId="47"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="2" xr9:uid="{04D63829-0BD7-4440-A6B4-835A3AD8C080}">
-      <tableStyleElement type="wholeTable" dxfId="47"/>
-      <tableStyleElement type="headerRow" dxfId="46"/>
+      <tableStyleElement type="wholeTable" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="45"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -931,8 +923,8 @@
       <xdr:rowOff>24375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>56808</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1544522</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>152368</xdr:rowOff>
     </xdr:to>
@@ -1027,14 +1019,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA289B82-93BA-4660-8B80-AC950692FB06}" name="DatosPersonales" displayName="DatosPersonales" ref="A10:L11" headerRowDxfId="45" dataDxfId="43" headerRowBorderDxfId="44" tableBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA289B82-93BA-4660-8B80-AC950692FB06}" name="DatosPersonales" displayName="DatosPersonales" ref="A10:L11" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41">
   <autoFilter ref="A10:L11" xr:uid="{FA289B82-93BA-4660-8B80-AC950692FB06}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{424FEB43-7374-4B09-B25E-3B08E53232EF}" name="N°" totalsRowLabel="Total" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{D053C162-9DF9-446F-B9E7-A9DF0D2AC0B5}" name="Nombre Completo" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{90409209-5CC9-424E-843A-B05D69B48CFC}" name="Identificación" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{AC555016-E08F-4DDA-AEE7-8DB116B15AE9}" name="Tipo de Identificación" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{A3DB3350-F537-40E8-AD4C-C1061652733E}" name="País" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{424FEB43-7374-4B09-B25E-3B08E53232EF}" name="N°" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{D053C162-9DF9-446F-B9E7-A9DF0D2AC0B5}" name="Nombre Completo" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{90409209-5CC9-424E-843A-B05D69B48CFC}" name="Identificación" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{AC555016-E08F-4DDA-AEE7-8DB116B15AE9}" name="Tipo de Identificación" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{A3DB3350-F537-40E8-AD4C-C1061652733E}" name="País" dataDxfId="32"/>
     <tableColumn id="6" xr3:uid="{451100BF-9CDB-45FC-8CAF-5FD52DCC0F83}" name="Sexo" dataDxfId="31" totalsRowDxfId="30"/>
     <tableColumn id="7" xr3:uid="{83E5905F-35F6-49EA-82B4-F14EDA73A729}" name="Fecha de Nacimiento" dataDxfId="29" totalsRowDxfId="28"/>
     <tableColumn id="8" xr3:uid="{9D4BC2B9-A3BC-4533-AE0C-9B5DBFBB548C}" name="Edad" dataDxfId="27" totalsRowDxfId="26"/>
@@ -1059,7 +1051,7 @@
     <tableColumn id="6" xr3:uid="{86E05F0C-1357-4680-B887-9B7D8095A907}" name="Motivos de Salida del País" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{F4BCF7FC-E598-47CF-9463-BD07E927B3DC}" name="Necesidades que Presenta" dataDxfId="7"/>
     <tableColumn id="8" xr3:uid="{F8C7D026-897E-4792-BCC1-BBF197F7B309}" name="Discapacidades" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{08FBB0A7-703D-4C2E-BF28-96394B912FD7}" name="Fallecimiento" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{08FBB0A7-703D-4C2E-BF28-96394B912FD7}" name="Falleció" dataDxfId="5"/>
     <tableColumn id="10" xr3:uid="{64A66704-78ED-46AA-83B7-F6CF4377D55E}" name="Atención Psicológica" dataDxfId="4"/>
     <tableColumn id="11" xr3:uid="{993D0DFC-AA55-4AD0-AE87-D43D7DB84B7A}" name="Asesoría Psicológica" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{10C49B21-2149-4C03-AE5E-16DEDA43BE1C}" name="Atención Legal" dataDxfId="2"/>
@@ -1335,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="T4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1345,7 +1337,7 @@
     <col min="2" max="2" width="48.7265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="29.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.6328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="25" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.54296875" style="1" customWidth="1"/>
@@ -1356,89 +1348,89 @@
     <col min="13" max="13" width="24.1796875" style="1" customWidth="1"/>
     <col min="14" max="14" width="22.453125" style="1" customWidth="1"/>
     <col min="15" max="15" width="24.7265625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="19.1796875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="22.54296875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.54296875" style="1" customWidth="1"/>
     <col min="18" max="18" width="37.90625" style="1" customWidth="1"/>
     <col min="19" max="19" width="32.453125" style="1" customWidth="1"/>
     <col min="20" max="20" width="30.26953125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.54296875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="24.08984375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="21.90625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="19.6328125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="21.7265625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.90625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="27" style="1" customWidth="1"/>
+    <col min="23" max="23" width="26.453125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="22.08984375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="26" style="1" customWidth="1"/>
     <col min="26" max="26" width="25.453125" style="1" customWidth="1"/>
     <col min="27" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+    <row r="1" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10"/>
+    <row r="3" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10"/>
+    <row r="4" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10"/>
+    <row r="5" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
+    <row r="6" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+    <row r="7" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:40" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
@@ -1455,14 +1447,14 @@
       <c r="AN9" s="2"/>
     </row>
     <row r="10" spans="1:40" s="4" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>3</v>
@@ -1516,22 +1508,22 @@
         <v>19</v>
       </c>
       <c r="U10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="W10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="X10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y10" s="3" t="s">
+      <c r="Z10" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglado valor en notacion cientifica en numero de identificacion en generar excel
</commit_message>
<xml_diff>
--- a/registros/plantilla/plantilla_registro_atenciones.xlsx
+++ b/registros/plantilla/plantilla_registro_atenciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRM-CARITAS\registros\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85277854-9DB4-4FFB-B41D-C956680CA015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DD026E-EF91-4BB1-B8BA-8ED25F7E432C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Migrantes" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -355,11 +355,25 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -528,14 +542,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1024,39 +1030,39 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{424FEB43-7374-4B09-B25E-3B08E53232EF}" name="N°" totalsRowLabel="Total" dataDxfId="40" totalsRowDxfId="39"/>
     <tableColumn id="2" xr3:uid="{D053C162-9DF9-446F-B9E7-A9DF0D2AC0B5}" name="Nombre Completo" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{90409209-5CC9-424E-843A-B05D69B48CFC}" name="Identificación" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{AC555016-E08F-4DDA-AEE7-8DB116B15AE9}" name="Tipo de Identificación" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{A3DB3350-F537-40E8-AD4C-C1061652733E}" name="País" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{451100BF-9CDB-45FC-8CAF-5FD52DCC0F83}" name="Sexo" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{83E5905F-35F6-49EA-82B4-F14EDA73A729}" name="Fecha de Nacimiento" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{9D4BC2B9-A3BC-4533-AE0C-9B5DBFBB548C}" name="Edad" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{158BD100-B55F-4262-A4A8-FE65B97DEEAD}" name="Estado Civil" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{DD6211FA-90C8-4ED1-838A-589D5453AA95}" name="Código Familiar" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{FE54DF5A-0F08-4DA3-88C2-5C830ED68000}" name="¿Es LGBT?" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{CC163A24-DC7D-4A4E-9AFE-4AE0B3909A09}" name="Tipo de Sangre" totalsRowFunction="count" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{90409209-5CC9-424E-843A-B05D69B48CFC}" name="Identificación" dataDxfId="0" totalsRowDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{AC555016-E08F-4DDA-AEE7-8DB116B15AE9}" name="Tipo de Identificación" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{A3DB3350-F537-40E8-AD4C-C1061652733E}" name="País" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{451100BF-9CDB-45FC-8CAF-5FD52DCC0F83}" name="Sexo" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{83E5905F-35F6-49EA-82B4-F14EDA73A729}" name="Fecha de Nacimiento" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{9D4BC2B9-A3BC-4533-AE0C-9B5DBFBB548C}" name="Edad" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{158BD100-B55F-4262-A4A8-FE65B97DEEAD}" name="Estado Civil" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{DD6211FA-90C8-4ED1-838A-589D5453AA95}" name="Código Familiar" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{FE54DF5A-0F08-4DA3-88C2-5C830ED68000}" name="¿Es LGBT?" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{CC163A24-DC7D-4A4E-9AFE-4AE0B3909A09}" name="Tipo de Sangre" totalsRowFunction="count" dataDxfId="20" totalsRowDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5F5D2341-15B3-4788-A833-5AFB3B690C38}" name="Expedientes" displayName="Expedientes" ref="M10:Z11" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5F5D2341-15B3-4788-A833-5AFB3B690C38}" name="Expedientes" displayName="Expedientes" ref="M10:Z11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15">
   <autoFilter ref="M10:Z11" xr:uid="{5F5D2341-15B3-4788-A833-5AFB3B690C38}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2F6FAC9A-3F12-427E-AF8A-EE8C7F00DAE4}" name="Situación Migratoria" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{944EF00B-5D38-498D-845B-E615388D0D09}" name="Frontera" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{6530FC45-9616-4468-ABCD-AB976F032B62}" name="Asesor Migratorio" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{2213E729-1CA0-4FF3-BC6C-A090031C2439}" name="Fecha de Ingreso" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{5D9703E6-37B4-4861-A2E4-6255EA62F742}" name="Fecha de Salida" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{86E05F0C-1357-4680-B887-9B7D8095A907}" name="Motivos de Salida del País" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{F4BCF7FC-E598-47CF-9463-BD07E927B3DC}" name="Necesidades que Presenta" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{F8C7D026-897E-4792-BCC1-BBF197F7B309}" name="Discapacidades" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{08FBB0A7-703D-4C2E-BF28-96394B912FD7}" name="Falleció" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{64A66704-78ED-46AA-83B7-F6CF4377D55E}" name="Atención Psicológica" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{993D0DFC-AA55-4AD0-AE87-D43D7DB84B7A}" name="Asesoría Psicológica" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{10C49B21-2149-4C03-AE5E-16DEDA43BE1C}" name="Atención Legal" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{6CB7BDAD-0B23-4B98-8771-0911E4E4B596}" name="Asesoría Psicosocial" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{4012B120-A973-4426-888B-25BFBCBD8E5F}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2F6FAC9A-3F12-427E-AF8A-EE8C7F00DAE4}" name="Situación Migratoria" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{944EF00B-5D38-498D-845B-E615388D0D09}" name="Frontera" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{6530FC45-9616-4468-ABCD-AB976F032B62}" name="Asesor Migratorio" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{2213E729-1CA0-4FF3-BC6C-A090031C2439}" name="Fecha de Ingreso" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{5D9703E6-37B4-4861-A2E4-6255EA62F742}" name="Fecha de Salida" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{86E05F0C-1357-4680-B887-9B7D8095A907}" name="Motivos de Salida del País" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{F4BCF7FC-E598-47CF-9463-BD07E927B3DC}" name="Necesidades que Presenta" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{F8C7D026-897E-4792-BCC1-BBF197F7B309}" name="Discapacidades" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{08FBB0A7-703D-4C2E-BF28-96394B912FD7}" name="Falleció" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{64A66704-78ED-46AA-83B7-F6CF4377D55E}" name="Atención Psicológica" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{993D0DFC-AA55-4AD0-AE87-D43D7DB84B7A}" name="Asesoría Psicológica" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{10C49B21-2149-4C03-AE5E-16DEDA43BE1C}" name="Atención Legal" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{6CB7BDAD-0B23-4B98-8771-0911E4E4B596}" name="Asesoría Psicosocial" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{4012B120-A973-4426-888B-25BFBCBD8E5F}" name="Observaciones" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1327,15 +1333,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" style="15" customWidth="1"/>
     <col min="4" max="4" width="29.08984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.54296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.6328125" style="1" customWidth="1"/>
@@ -1362,7 +1368,9 @@
     <col min="27" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="13"/>
+    </row>
     <row r="2" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>26</v>
@@ -1399,7 +1407,9 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:40" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="13"/>
+    </row>
     <row r="9" spans="1:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>11</v>
@@ -1453,7 +1463,7 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">

</xml_diff>